<commit_message>
Fixed incorrect SMILES string for step 1 product in manual bis(2-bromophenyl)dimethylsilane synthesis.
</commit_message>
<xml_diff>
--- a/Rxn_Summs/bis(2-bromophenyl)dimethylsilane.xlsx
+++ b/Rxn_Summs/bis(2-bromophenyl)dimethylsilane.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mseifrid/Dropbox (Aspuru-Guzik Lab)/Matter Lab/Projects/Subway synthesis/testing/Rxn_Summs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mseifrid/Dropbox (Aspuru-Guzik Lab)/Matter Lab/Data/Code/Subway_Maps/Rxn_Summs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E43D751-6EDC-EE49-AF48-92E06539C6AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26332C34-612B-4F4F-BF15-D0AF7DE13B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17900" yWindow="460" windowWidth="17920" windowHeight="21940" activeTab="1" xr2:uid="{010DAFF7-FEB8-624D-A540-AEB035FC1AFC}"/>
+    <workbookView xWindow="17900" yWindow="460" windowWidth="17920" windowHeight="21940" xr2:uid="{010DAFF7-FEB8-624D-A540-AEB035FC1AFC}"/>
   </bookViews>
   <sheets>
     <sheet name="step 1" sheetId="1" r:id="rId1"/>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37651B9D-A9E5-D744-9A8E-85A3C559FC2E}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -546,7 +546,7 @@
         <v>0.87</v>
       </c>
       <c r="L2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -566,7 +566,7 @@
         <v>38.9</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F4" si="0">C3*(E3/D3)</f>
+        <f t="shared" ref="F3" si="0">C3*(E3/D3)</f>
         <v>40.494723981900449</v>
       </c>
       <c r="G3">
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A5FA00-367C-A845-8DD4-707462578352}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>